<commit_message>
Added Worked Hours In Employee Schedule table
</commit_message>
<xml_diff>
--- a/config_files/Horarios/Palobiofarma, S.L Mataró/Ivette Amalfi.xlsx
+++ b/config_files/Horarios/Palobiofarma, S.L Mataró/Ivette Amalfi.xlsx
@@ -5703,7 +5703,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="490">
+  <cellXfs count="492">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true"/>
     <xf xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
@@ -6839,6 +6839,12 @@
     </xf>
     <xf xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:main="http://schemas.openxmlformats.org/spreadsheetml/2006/main" numFmtId="0" fontId="489" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="1" applyFill="true" applyBorder="true" applyNumberFormat="true">
       <main:alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
 </styleSheet>
@@ -7368,36 +7374,36 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" customWidth="true"/>
-    <col min="2" max="2" width="6.77734375" customWidth="true"/>
-    <col min="3" max="3" width="6.77734375" customWidth="true"/>
-    <col min="4" max="4" width="6.77734375" customWidth="true"/>
-    <col min="5" max="5" width="6.77734375" customWidth="true"/>
-    <col min="6" max="6" width="6.77734375" customWidth="true"/>
-    <col min="7" max="7" width="6.77734375" customWidth="true"/>
-    <col min="8" max="8" width="6.77734375" customWidth="true"/>
-    <col min="9" max="9" width="2.77734375" customWidth="true"/>
-    <col min="10" max="10" width="6.77734375" customWidth="true"/>
-    <col min="11" max="11" width="6.77734375" customWidth="true"/>
-    <col min="12" max="12" width="6.77734375" customWidth="true"/>
-    <col min="13" max="13" width="6.77734375" customWidth="true"/>
-    <col min="14" max="14" width="6.77734375" customWidth="true"/>
-    <col min="15" max="15" width="6.77734375" customWidth="true"/>
-    <col min="16" max="16" width="6.77734375" customWidth="true"/>
-    <col min="17" max="17" width="2.77734375" customWidth="true"/>
-    <col min="18" max="18" width="6.77734375" customWidth="true"/>
-    <col min="19" max="19" width="6.77734375" customWidth="true"/>
-    <col min="20" max="20" width="6.77734375" customWidth="true"/>
-    <col min="21" max="21" width="6.77734375" customWidth="true"/>
-    <col min="22" max="22" width="6.77734375" customWidth="true"/>
-    <col min="23" max="23" width="6.77734375" customWidth="true"/>
-    <col min="24" max="24" width="6.77734375" customWidth="true"/>
-    <col min="25" max="25" width="10.0" customWidth="true"/>
-    <col min="26" max="26" width="6.0" customWidth="true"/>
-    <col min="27" max="27" width="21.77734375" customWidth="true"/>
-    <col min="28" max="28" width="21.77734375" customWidth="true"/>
-    <col min="29" max="29" width="21.77734375" customWidth="true"/>
-    <col min="30" max="30" width="10.0" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="2.77734375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="2.77734375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="2.77734375" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="6.77734375" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" width="6.0" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" width="21.77734375" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" width="21.77734375" collapsed="true"/>
+    <col min="29" max="29" customWidth="true" width="21.77734375" collapsed="true"/>
+    <col min="30" max="30" customWidth="true" width="10.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" ht="25.8" customHeight="true">
@@ -9391,23 +9397,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="true"/>
-    <col min="2" max="2" width="18.6640625" customWidth="true"/>
-    <col min="3" max="3" width="18.0" customWidth="true"/>
-    <col min="4" max="4" width="3.109375" customWidth="true"/>
-    <col min="5" max="5" width="18.6640625" customWidth="true"/>
-    <col min="6" max="6" width="3.109375" customWidth="true"/>
-    <col min="7" max="7" width="14.6640625" customWidth="true"/>
-    <col min="8" max="8" width="4.6640625" customWidth="true"/>
-    <col min="9" max="9" width="10.88671875" customWidth="true"/>
-    <col min="10" max="10" width="5.33203125" customWidth="true"/>
-    <col min="11" max="11" width="13.33203125" customWidth="true"/>
-    <col min="12" max="12" width="10.88671875" customWidth="true"/>
-    <col min="13" max="13" width="10.88671875" customWidth="true"/>
-    <col min="14" max="14" width="10.88671875" customWidth="true"/>
-    <col min="15" max="15" width="10.88671875" customWidth="true"/>
-    <col min="16" max="16" width="10.88671875" customWidth="true"/>
-    <col min="17" max="17" width="10.88671875" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -9987,23 +9993,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="true"/>
-    <col min="2" max="2" width="18.6640625" customWidth="true"/>
-    <col min="3" max="3" width="18.0" customWidth="true"/>
-    <col min="4" max="4" width="3.109375" customWidth="true"/>
-    <col min="5" max="5" width="18.6640625" customWidth="true"/>
-    <col min="6" max="6" width="3.109375" customWidth="true"/>
-    <col min="7" max="7" width="14.6640625" customWidth="true"/>
-    <col min="8" max="8" width="4.6640625" customWidth="true"/>
-    <col min="9" max="9" width="10.88671875" customWidth="true"/>
-    <col min="10" max="10" width="5.33203125" customWidth="true"/>
-    <col min="11" max="11" width="13.33203125" customWidth="true"/>
-    <col min="12" max="12" width="10.88671875" customWidth="true"/>
-    <col min="13" max="13" width="10.88671875" customWidth="true"/>
-    <col min="14" max="14" width="10.88671875" customWidth="true"/>
-    <col min="15" max="15" width="10.88671875" customWidth="true"/>
-    <col min="16" max="16" width="10.88671875" customWidth="true"/>
-    <col min="17" max="17" width="10.88671875" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -10590,23 +10596,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="true"/>
-    <col min="2" max="2" width="18.6640625" customWidth="true"/>
-    <col min="3" max="3" width="18.0" customWidth="true"/>
-    <col min="4" max="4" width="3.109375" customWidth="true"/>
-    <col min="5" max="5" width="18.6640625" customWidth="true"/>
-    <col min="6" max="6" width="3.109375" customWidth="true"/>
-    <col min="7" max="7" width="14.6640625" customWidth="true"/>
-    <col min="8" max="8" width="4.6640625" customWidth="true"/>
-    <col min="9" max="9" width="10.88671875" customWidth="true"/>
-    <col min="10" max="10" width="5.33203125" customWidth="true"/>
-    <col min="11" max="11" width="13.33203125" customWidth="true"/>
-    <col min="12" max="12" width="10.88671875" customWidth="true"/>
-    <col min="13" max="13" width="10.88671875" customWidth="true"/>
-    <col min="14" max="14" width="10.88671875" customWidth="true"/>
-    <col min="15" max="15" width="10.88671875" customWidth="true"/>
-    <col min="16" max="16" width="10.88671875" customWidth="true"/>
-    <col min="17" max="17" width="10.88671875" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -11185,23 +11191,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="true"/>
-    <col min="2" max="2" width="18.6640625" customWidth="true"/>
-    <col min="3" max="3" width="18.0" customWidth="true"/>
-    <col min="4" max="4" width="3.109375" customWidth="true"/>
-    <col min="5" max="5" width="18.6640625" customWidth="true"/>
-    <col min="6" max="6" width="3.109375" customWidth="true"/>
-    <col min="7" max="7" width="14.6640625" customWidth="true"/>
-    <col min="8" max="8" width="4.6640625" customWidth="true"/>
-    <col min="9" max="9" width="10.88671875" customWidth="true"/>
-    <col min="10" max="10" width="5.33203125" customWidth="true"/>
-    <col min="11" max="11" width="13.33203125" customWidth="true"/>
-    <col min="12" max="12" width="10.88671875" customWidth="true"/>
-    <col min="13" max="13" width="10.88671875" customWidth="true"/>
-    <col min="14" max="14" width="10.88671875" customWidth="true"/>
-    <col min="15" max="15" width="10.88671875" customWidth="true"/>
-    <col min="16" max="16" width="10.88671875" customWidth="true"/>
-    <col min="17" max="17" width="10.88671875" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -11787,23 +11793,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="true"/>
-    <col min="2" max="2" width="18.6640625" customWidth="true"/>
-    <col min="3" max="3" width="18.0" customWidth="true"/>
-    <col min="4" max="4" width="3.109375" customWidth="true"/>
-    <col min="5" max="5" width="18.6640625" customWidth="true"/>
-    <col min="6" max="6" width="3.109375" customWidth="true"/>
-    <col min="7" max="7" width="14.6640625" customWidth="true"/>
-    <col min="8" max="8" width="4.6640625" customWidth="true"/>
-    <col min="9" max="9" width="10.88671875" customWidth="true"/>
-    <col min="10" max="10" width="5.33203125" customWidth="true"/>
-    <col min="11" max="11" width="13.33203125" customWidth="true"/>
-    <col min="12" max="12" width="10.88671875" customWidth="true"/>
-    <col min="13" max="13" width="10.88671875" customWidth="true"/>
-    <col min="14" max="14" width="10.88671875" customWidth="true"/>
-    <col min="15" max="15" width="10.88671875" customWidth="true"/>
-    <col min="16" max="16" width="10.88671875" customWidth="true"/>
-    <col min="17" max="17" width="10.88671875" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -11982,8 +11988,12 @@
       <c r="B18" s="127" t="n">
         <v>3.0</v>
       </c>
-      <c r="C18" s="128"/>
-      <c r="E18" s="128"/>
+      <c r="C18" s="491" t="n">
+        <v>0.3541666666666667</v>
+      </c>
+      <c r="E18" s="491" t="n">
+        <v>0.7291666666666666</v>
+      </c>
       <c r="G18" s="125" t="n">
         <f>((E18-C18)*24)-1</f>
         <v>0.0</v>
@@ -11993,8 +12003,12 @@
       <c r="B19" s="127" t="n">
         <v>4.0</v>
       </c>
-      <c r="C19" s="128"/>
-      <c r="E19" s="128"/>
+      <c r="C19" s="491" t="n">
+        <v>0.3854166666666667</v>
+      </c>
+      <c r="E19" s="491" t="n">
+        <v>0.7604166666666666</v>
+      </c>
       <c r="G19" s="125" t="n">
         <f>((E19-C19)*24)-1</f>
         <v>0.0</v>
@@ -12004,8 +12018,12 @@
       <c r="B20" s="127" t="n">
         <v>5.0</v>
       </c>
-      <c r="C20" s="128"/>
-      <c r="E20" s="128"/>
+      <c r="C20" s="491" t="n">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="E20" s="491" t="n">
+        <v>0.7638888888888888</v>
+      </c>
       <c r="G20" s="125" t="n">
         <f>((E20-C20)*24)-1</f>
         <v>0.0</v>
@@ -12025,8 +12043,12 @@
       <c r="B22" s="127" t="n">
         <v>7.0</v>
       </c>
-      <c r="C22" s="128"/>
-      <c r="E22" s="128"/>
+      <c r="C22" s="491" t="n">
+        <v>0.34375</v>
+      </c>
+      <c r="E22" s="491" t="n">
+        <v>0.71875</v>
+      </c>
       <c r="G22" s="125" t="n">
         <f>((E22-C22)*24)-1</f>
         <v>0.0</v>
@@ -12056,8 +12078,12 @@
       <c r="B25" s="127" t="n">
         <v>10.0</v>
       </c>
-      <c r="C25" s="128"/>
-      <c r="E25" s="128"/>
+      <c r="C25" s="491" t="n">
+        <v>0.3576388888888889</v>
+      </c>
+      <c r="E25" s="491" t="n">
+        <v>0.7326388888888888</v>
+      </c>
       <c r="G25" s="125" t="n">
         <f>((E25-C25)*24)-1</f>
         <v>0.0</v>
@@ -12067,8 +12093,12 @@
       <c r="B26" s="127" t="n">
         <v>11.0</v>
       </c>
-      <c r="C26" s="128"/>
-      <c r="E26" s="128"/>
+      <c r="C26" s="491" t="n">
+        <v>0.3402777777777778</v>
+      </c>
+      <c r="E26" s="491" t="n">
+        <v>0.7152777777777778</v>
+      </c>
       <c r="G26" s="125" t="n">
         <f>((E26-C26)*24)-1</f>
         <v>0.0</v>
@@ -12078,8 +12108,12 @@
       <c r="B27" s="127" t="n">
         <v>12.0</v>
       </c>
-      <c r="C27" s="128"/>
-      <c r="E27" s="128"/>
+      <c r="C27" s="491" t="n">
+        <v>0.3506944444444444</v>
+      </c>
+      <c r="E27" s="491" t="n">
+        <v>0.7256944444444444</v>
+      </c>
       <c r="G27" s="125" t="n">
         <f>((E27-C27)*24)-1</f>
         <v>0.0</v>
@@ -12089,8 +12123,12 @@
       <c r="B28" s="127" t="n">
         <v>13.0</v>
       </c>
-      <c r="C28" s="128"/>
-      <c r="E28" s="128"/>
+      <c r="C28" s="491" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E28" s="491" t="n">
+        <v>0.75</v>
+      </c>
       <c r="G28" s="125" t="n">
         <f>((E28-C28)*24)-1</f>
         <v>0.0</v>
@@ -12100,8 +12138,12 @@
       <c r="B29" s="127" t="n">
         <v>14.0</v>
       </c>
-      <c r="C29" s="128"/>
-      <c r="E29" s="128"/>
+      <c r="C29" s="491" t="n">
+        <v>0.3770833333333333</v>
+      </c>
+      <c r="E29" s="491" t="n">
+        <v>0.7520833333333333</v>
+      </c>
       <c r="G29" s="125" t="n">
         <f>((E29-C29)*24)-1</f>
         <v>0.0</v>
@@ -12131,8 +12173,12 @@
       <c r="B32" s="127" t="n">
         <v>17.0</v>
       </c>
-      <c r="C32" s="128"/>
-      <c r="E32" s="128"/>
+      <c r="C32" s="491" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E32" s="491" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G32" s="125" t="n">
         <f>((E32-C32)*24)-1</f>
         <v>0.0</v>
@@ -12142,8 +12188,12 @@
       <c r="B33" s="127" t="n">
         <v>18.0</v>
       </c>
-      <c r="C33" s="128"/>
-      <c r="E33" s="128"/>
+      <c r="C33" s="491" t="n">
+        <v>0.3402777777777778</v>
+      </c>
+      <c r="E33" s="491" t="n">
+        <v>0.7152777777777778</v>
+      </c>
       <c r="G33" s="125" t="n">
         <f>((E33-C33)*24)-1</f>
         <v>0.0</v>
@@ -12153,8 +12203,12 @@
       <c r="B34" s="127" t="n">
         <v>19.0</v>
       </c>
-      <c r="C34" s="128"/>
-      <c r="E34" s="128"/>
+      <c r="C34" s="491" t="n">
+        <v>0.3854166666666667</v>
+      </c>
+      <c r="E34" s="491" t="n">
+        <v>0.7604166666666666</v>
+      </c>
       <c r="G34" s="125" t="n">
         <f>((E34-C34)*24)-1</f>
         <v>0.0</v>
@@ -12164,8 +12218,12 @@
       <c r="B35" s="127" t="n">
         <v>20.0</v>
       </c>
-      <c r="C35" s="128"/>
-      <c r="E35" s="128"/>
+      <c r="C35" s="491" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E35" s="491" t="n">
+        <v>0.75</v>
+      </c>
       <c r="G35" s="125" t="n">
         <f>((E35-C35)*24)-1</f>
         <v>0.0</v>
@@ -12175,8 +12233,12 @@
       <c r="B36" s="127" t="n">
         <v>21.0</v>
       </c>
-      <c r="C36" s="128"/>
-      <c r="E36" s="128"/>
+      <c r="C36" s="491" t="n">
+        <v>0.3541666666666667</v>
+      </c>
+      <c r="E36" s="491" t="n">
+        <v>0.7291666666666666</v>
+      </c>
       <c r="G36" s="125" t="n">
         <f>((E36-C36)*24)-1</f>
         <v>0.0</v>
@@ -12206,8 +12268,12 @@
       <c r="B39" s="127" t="n">
         <v>24.0</v>
       </c>
-      <c r="C39" s="128"/>
-      <c r="E39" s="128"/>
+      <c r="C39" s="491" t="n">
+        <v>0.40625</v>
+      </c>
+      <c r="E39" s="491" t="n">
+        <v>0.78125</v>
+      </c>
       <c r="G39" s="125" t="n">
         <f>((E39-C39)*24)-1</f>
         <v>0.0</v>
@@ -12217,8 +12283,12 @@
       <c r="B40" s="127" t="n">
         <v>25.0</v>
       </c>
-      <c r="C40" s="128"/>
-      <c r="E40" s="128"/>
+      <c r="C40" s="491" t="n">
+        <v>0.3402777777777778</v>
+      </c>
+      <c r="E40" s="491" t="n">
+        <v>0.7152777777777778</v>
+      </c>
       <c r="G40" s="125" t="n">
         <f>((E40-C40)*24)-1</f>
         <v>0.0</v>
@@ -12228,8 +12298,12 @@
       <c r="B41" s="127" t="n">
         <v>26.0</v>
       </c>
-      <c r="C41" s="128"/>
-      <c r="E41" s="128"/>
+      <c r="C41" s="491" t="n">
+        <v>0.3958333333333333</v>
+      </c>
+      <c r="E41" s="491" t="n">
+        <v>0.7708333333333334</v>
+      </c>
       <c r="G41" s="125" t="n">
         <f>((E41-C41)*24)-1</f>
         <v>0.0</v>
@@ -12239,8 +12313,12 @@
       <c r="B42" s="127" t="n">
         <v>27.0</v>
       </c>
-      <c r="C42" s="128"/>
-      <c r="E42" s="128"/>
+      <c r="C42" s="491" t="n">
+        <v>0.3506944444444444</v>
+      </c>
+      <c r="E42" s="491" t="n">
+        <v>0.7256944444444444</v>
+      </c>
       <c r="G42" s="125" t="n">
         <f>((E42-C42)*24)-1</f>
         <v>0.0</v>
@@ -12250,8 +12328,12 @@
       <c r="B43" s="127" t="n">
         <v>28.0</v>
       </c>
-      <c r="C43" s="128"/>
-      <c r="E43" s="128"/>
+      <c r="C43" s="491" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E43" s="491" t="n">
+        <v>0.75</v>
+      </c>
       <c r="G43" s="125" t="n">
         <f>((E43-C43)*24)-1</f>
         <v>0.0</v>
@@ -12281,8 +12363,12 @@
       <c r="B46" s="127" t="n">
         <v>31.0</v>
       </c>
-      <c r="C46" s="128"/>
-      <c r="E46" s="128"/>
+      <c r="C46" s="491" t="n">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E46" s="491" t="n">
+        <v>0.7083333333333334</v>
+      </c>
       <c r="G46" s="125" t="n">
         <f>((E46-C46)*24)-1</f>
         <v>0.0</v>
@@ -12411,23 +12497,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="true"/>
-    <col min="2" max="2" width="18.6640625" customWidth="true"/>
-    <col min="3" max="3" width="18.0" customWidth="true"/>
-    <col min="4" max="4" width="3.109375" customWidth="true"/>
-    <col min="5" max="5" width="18.6640625" customWidth="true"/>
-    <col min="6" max="6" width="3.109375" customWidth="true"/>
-    <col min="7" max="7" width="14.6640625" customWidth="true"/>
-    <col min="8" max="8" width="4.6640625" customWidth="true"/>
-    <col min="9" max="9" width="10.88671875" customWidth="true"/>
-    <col min="10" max="10" width="5.33203125" customWidth="true"/>
-    <col min="11" max="11" width="13.33203125" customWidth="true"/>
-    <col min="12" max="12" width="10.88671875" customWidth="true"/>
-    <col min="13" max="13" width="10.88671875" customWidth="true"/>
-    <col min="14" max="14" width="10.88671875" customWidth="true"/>
-    <col min="15" max="15" width="10.88671875" customWidth="true"/>
-    <col min="16" max="16" width="10.88671875" customWidth="true"/>
-    <col min="17" max="17" width="10.88671875" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -13020,23 +13106,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="true"/>
-    <col min="2" max="2" width="18.6640625" customWidth="true"/>
-    <col min="3" max="3" width="18.0" customWidth="true"/>
-    <col min="4" max="4" width="3.109375" customWidth="true"/>
-    <col min="5" max="5" width="18.6640625" customWidth="true"/>
-    <col min="6" max="6" width="3.109375" customWidth="true"/>
-    <col min="7" max="7" width="14.6640625" customWidth="true"/>
-    <col min="8" max="8" width="4.6640625" customWidth="true"/>
-    <col min="9" max="9" width="10.88671875" customWidth="true"/>
-    <col min="10" max="10" width="5.33203125" customWidth="true"/>
-    <col min="11" max="11" width="13.33203125" customWidth="true"/>
-    <col min="12" max="12" width="10.88671875" customWidth="true"/>
-    <col min="13" max="13" width="10.88671875" customWidth="true"/>
-    <col min="14" max="14" width="10.88671875" customWidth="true"/>
-    <col min="15" max="15" width="10.88671875" customWidth="true"/>
-    <col min="16" max="16" width="10.88671875" customWidth="true"/>
-    <col min="17" max="17" width="10.88671875" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -13641,23 +13727,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="true"/>
-    <col min="2" max="2" width="18.6640625" customWidth="true"/>
-    <col min="3" max="3" width="18.0" customWidth="true"/>
-    <col min="4" max="4" width="3.109375" customWidth="true"/>
-    <col min="5" max="5" width="18.6640625" customWidth="true"/>
-    <col min="6" max="6" width="3.109375" customWidth="true"/>
-    <col min="7" max="7" width="14.6640625" customWidth="true"/>
-    <col min="8" max="8" width="4.6640625" customWidth="true"/>
-    <col min="9" max="9" width="10.88671875" customWidth="true"/>
-    <col min="10" max="10" width="5.33203125" customWidth="true"/>
-    <col min="11" max="11" width="13.33203125" customWidth="true"/>
-    <col min="12" max="12" width="10.88671875" customWidth="true"/>
-    <col min="13" max="13" width="10.88671875" customWidth="true"/>
-    <col min="14" max="14" width="10.88671875" customWidth="true"/>
-    <col min="15" max="15" width="10.88671875" customWidth="true"/>
-    <col min="16" max="16" width="10.88671875" customWidth="true"/>
-    <col min="17" max="17" width="10.88671875" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -14253,23 +14339,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="true"/>
-    <col min="2" max="2" width="18.6640625" customWidth="true"/>
-    <col min="3" max="3" width="18.0" customWidth="true"/>
-    <col min="4" max="4" width="3.109375" customWidth="true"/>
-    <col min="5" max="5" width="18.6640625" customWidth="true"/>
-    <col min="6" max="6" width="3.109375" customWidth="true"/>
-    <col min="7" max="7" width="14.6640625" customWidth="true"/>
-    <col min="8" max="8" width="4.6640625" customWidth="true"/>
-    <col min="9" max="9" width="10.88671875" customWidth="true"/>
-    <col min="10" max="10" width="5.33203125" customWidth="true"/>
-    <col min="11" max="11" width="13.33203125" customWidth="true"/>
-    <col min="12" max="12" width="10.88671875" customWidth="true"/>
-    <col min="13" max="13" width="10.88671875" customWidth="true"/>
-    <col min="14" max="14" width="10.88671875" customWidth="true"/>
-    <col min="15" max="15" width="10.88671875" customWidth="true"/>
-    <col min="16" max="16" width="10.88671875" customWidth="true"/>
-    <col min="17" max="17" width="10.88671875" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -14873,23 +14959,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="true"/>
-    <col min="2" max="2" width="18.6640625" customWidth="true"/>
-    <col min="3" max="3" width="18.0" customWidth="true"/>
-    <col min="4" max="4" width="3.109375" customWidth="true"/>
-    <col min="5" max="5" width="18.6640625" customWidth="true"/>
-    <col min="6" max="6" width="3.109375" customWidth="true"/>
-    <col min="7" max="7" width="14.6640625" customWidth="true"/>
-    <col min="8" max="8" width="4.6640625" customWidth="true"/>
-    <col min="9" max="9" width="10.88671875" customWidth="true"/>
-    <col min="10" max="10" width="5.33203125" customWidth="true"/>
-    <col min="11" max="11" width="13.33203125" customWidth="true"/>
-    <col min="12" max="12" width="10.88671875" customWidth="true"/>
-    <col min="13" max="13" width="10.88671875" customWidth="true"/>
-    <col min="14" max="14" width="10.88671875" customWidth="true"/>
-    <col min="15" max="15" width="10.88671875" customWidth="true"/>
-    <col min="16" max="16" width="10.88671875" customWidth="true"/>
-    <col min="17" max="17" width="10.88671875" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -15471,23 +15557,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="true"/>
-    <col min="2" max="2" width="18.6640625" customWidth="true"/>
-    <col min="3" max="3" width="18.0" customWidth="true"/>
-    <col min="4" max="4" width="3.109375" customWidth="true"/>
-    <col min="5" max="5" width="18.6640625" customWidth="true"/>
-    <col min="6" max="6" width="3.109375" customWidth="true"/>
-    <col min="7" max="7" width="14.6640625" customWidth="true"/>
-    <col min="8" max="8" width="4.6640625" customWidth="true"/>
-    <col min="9" max="9" width="10.88671875" customWidth="true"/>
-    <col min="10" max="10" width="5.33203125" customWidth="true"/>
-    <col min="11" max="11" width="13.33203125" customWidth="true"/>
-    <col min="12" max="12" width="10.88671875" customWidth="true"/>
-    <col min="13" max="13" width="10.88671875" customWidth="true"/>
-    <col min="14" max="14" width="10.88671875" customWidth="true"/>
-    <col min="15" max="15" width="10.88671875" customWidth="true"/>
-    <col min="16" max="16" width="10.88671875" customWidth="true"/>
-    <col min="17" max="17" width="10.88671875" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">
@@ -16073,23 +16159,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" customWidth="true"/>
-    <col min="2" max="2" width="18.6640625" customWidth="true"/>
-    <col min="3" max="3" width="18.0" customWidth="true"/>
-    <col min="4" max="4" width="3.109375" customWidth="true"/>
-    <col min="5" max="5" width="18.6640625" customWidth="true"/>
-    <col min="6" max="6" width="3.109375" customWidth="true"/>
-    <col min="7" max="7" width="14.6640625" customWidth="true"/>
-    <col min="8" max="8" width="4.6640625" customWidth="true"/>
-    <col min="9" max="9" width="10.88671875" customWidth="true"/>
-    <col min="10" max="10" width="5.33203125" customWidth="true"/>
-    <col min="11" max="11" width="13.33203125" customWidth="true"/>
-    <col min="12" max="12" width="10.88671875" customWidth="true"/>
-    <col min="13" max="13" width="10.88671875" customWidth="true"/>
-    <col min="14" max="14" width="10.88671875" customWidth="true"/>
-    <col min="15" max="15" width="10.88671875" customWidth="true"/>
-    <col min="16" max="16" width="10.88671875" customWidth="true"/>
-    <col min="17" max="17" width="10.88671875" customWidth="true"/>
+    <col min="1" max="1" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="3.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="4.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="5.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="10.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" ht="14.4" customHeight="true">

</xml_diff>